<commit_message>
Update Análise do aumento de consumo de memória.xlsx
</commit_message>
<xml_diff>
--- a/Files/Trabalhos/PA2/Análise do aumento de consumo de memória.xlsx
+++ b/Files/Trabalhos/PA2/Análise do aumento de consumo de memória.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\UFMG\Disciplinas\DCC831-TECC_Recuperacao_de_Informacao\Files\Trabalhos\PA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88806CB3-C5F8-4B87-9906-C3C6A87DF976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF644A2-E55B-481C-9B60-45B7BDD45BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{68C44311-49B4-4024-8D53-AA05B7B5CC92}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{68C44311-49B4-4024-8D53-AA05B7B5CC92}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -18079,12 +18080,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77587A3B-C25E-4D6E-ABBA-BB50509DBA6E}" name="Tabela1" displayName="Tabela1" ref="B1:D536" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77587A3B-C25E-4D6E-ABBA-BB50509DBA6E}" name="Tabela1" displayName="Tabela1" ref="B1:D536" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="B1:D536" xr:uid="{77587A3B-C25E-4D6E-ABBA-BB50509DBA6E}"/>
   <tableColumns count="3">
-    <tableColumn id="6" xr3:uid="{16968B8A-3956-4F18-92A5-8BF1AB975083}" name="#" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{42C71CDE-E1F0-40E0-8C38-A44E4397CA0D}" name="Pcss" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{954BDA08-4179-49DB-A3A0-D5374661F446}" name="Tot" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{16968B8A-3956-4F18-92A5-8BF1AB975083}" name="#" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{42C71CDE-E1F0-40E0-8C38-A44E4397CA0D}" name="Pcss" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{954BDA08-4179-49DB-A3A0-D5374661F446}" name="Tot" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18389,7 +18390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1B9083-896E-446D-B01D-2023A2D511E4}">
   <dimension ref="A1:I536"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -30729,54 +30730,6 @@
   </sheetData>
   <conditionalFormatting sqref="C2:C536">
     <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D536">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:I536">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:I536">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:I536">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30811,10 +30764,70 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D536">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:I536">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:I536">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1951AEAF-1B86-4517-AB5A-EDA86714DCF7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>